<commit_message>
Optimize the Xlsx2Ifc generator for product libraries #41
</commit_message>
<xml_diff>
--- a/SampleFiles/TriluxLightingProducts/SourceDataFromPimSystem/TRILUX_Baselist_RH190520.xlsx
+++ b/SampleFiles/TriluxLightingProducts/SourceDataFromPimSystem/TRILUX_Baselist_RH190520.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\GitHub\buildingSMART\ProductData\SampleFiles\TriluxLightingProducts\SourceDataFromPimSystem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC5B3976-0699-4856-9FBB-0F071649D84B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA2AF7E4-81F6-48B0-8AE2-6BF4D5F6C100}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="396" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -12287,9 +12287,6 @@
     <t>buildingSMART International</t>
   </si>
   <si>
-    <t>Trilux Individual Data Template</t>
-  </si>
-  <si>
     <t>TRILUX GmbH &amp; Co. KG</t>
   </si>
   <si>
@@ -12297,6 +12294,9 @@
   </si>
   <si>
     <t>Product image, e.g. as a jpeg file</t>
+  </si>
+  <si>
+    <t>Trilux Individual Product Data Template</t>
   </si>
 </sst>
 </file>
@@ -12913,8 +12913,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4A07687-0D17-4D6E-8F6E-1C562F7CF42C}">
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -13525,10 +13525,10 @@
     </row>
     <row r="26" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A26" s="15" t="s">
-        <v>4085</v>
+        <v>4084</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>4084</v>
+        <v>4087</v>
       </c>
       <c r="C26" s="15" t="s">
         <v>2287</v>
@@ -13550,10 +13550,10 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="15" t="s">
-        <v>4085</v>
+        <v>4084</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>4084</v>
+        <v>4087</v>
       </c>
       <c r="C27" s="15" t="s">
         <v>2279</v>
@@ -13573,16 +13573,16 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="15" t="s">
-        <v>4085</v>
+        <v>4084</v>
       </c>
       <c r="B28" s="15" t="s">
-        <v>4084</v>
+        <v>4087</v>
       </c>
       <c r="C28" s="15" t="s">
         <v>2296</v>
       </c>
       <c r="D28" s="19" t="s">
-        <v>4086</v>
+        <v>4085</v>
       </c>
       <c r="E28" s="15" t="s">
         <v>3161</v>
@@ -13596,16 +13596,16 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="15" t="s">
-        <v>4085</v>
+        <v>4084</v>
       </c>
       <c r="B29" s="15" t="s">
-        <v>4084</v>
+        <v>4087</v>
       </c>
       <c r="C29" s="15" t="s">
         <v>2295</v>
       </c>
       <c r="D29" s="19" t="s">
-        <v>4087</v>
+        <v>4086</v>
       </c>
       <c r="E29" s="15" t="s">
         <v>3160</v>

</xml_diff>